<commit_message>
Finalized git add . d d
</commit_message>
<xml_diff>
--- a/Model/Correlation/HyperParamIndices/Backtested.xlsx
+++ b/Model/Correlation/HyperParamIndices/Backtested.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Croissant\Internship\Yuanta\Model\Correlation\HyperParamIndices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chega/Desktop/Croissant/Internship/Yuanta-Intern/Model/Correlation/HyperParamIndices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4C3B9D-599E-4423-B5C8-460A1210F71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C7AA31-9F49-334E-BEF7-99F5B132A7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1000" windowWidth="19380" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,6 +123,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -560,33 +561,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" customWidth="1"/>
+    <col min="11" max="11" width="24.5" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="23.5" customWidth="1"/>
+    <col min="14" max="14" width="16.5" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" customWidth="1"/>
-    <col min="18" max="18" width="22.85546875" customWidth="1"/>
-    <col min="19" max="19" width="24.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" customWidth="1"/>
+    <col min="18" max="18" width="22.83203125" customWidth="1"/>
+    <col min="19" max="19" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -645,7 +646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -704,7 +705,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -760,7 +761,7 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -816,7 +817,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -872,7 +873,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -931,7 +932,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -987,7 +988,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1326,7 +1327,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1441,7 +1442,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1668,7 +1669,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1839,7 +1840,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1895,7 +1896,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2009,7 +2010,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D25">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2021,7 +2022,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G25">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2033,7 +2034,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L25">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2045,7 +2046,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O25">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>